<commit_message>
Resized board, added logo, rescaled trace size
</commit_message>
<xml_diff>
--- a/leak_sensor/LeakSensor_BOM.xlsx
+++ b/leak_sensor/LeakSensor_BOM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lane\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lane\Desktop\ARVP\au_hardware\leak_sensor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C18D343-58D3-4847-98DF-4544B6674E16}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F254B2E6-A3BD-4E9D-A6A8-0F2596FD177F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4410" xr2:uid="{9890E2C9-68FC-4E17-9560-E34A85D78A5C}"/>
   </bookViews>
@@ -148,9 +148,6 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -158,6 +155,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -477,7 +477,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,105 +491,105 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>0.65</v>
       </c>
-      <c r="F3" s="5">
-        <v>3</v>
-      </c>
-      <c r="G3" s="4">
-        <v>1.95</v>
+      <c r="F3" s="4">
+        <v>1</v>
+      </c>
+      <c r="G3" s="3">
+        <v>0.65</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>0.52</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>1</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>0.52</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>0.15</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>1</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>0.15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added filters and formatting to BOM
</commit_message>
<xml_diff>
--- a/leak_sensor/LeakSensor_BOM.xlsx
+++ b/leak_sensor/LeakSensor_BOM.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lane\Desktop\ARVP\au_hardware\leak_sensor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\Documents\Business\ARVP\au_hardware\leak_sensor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F254B2E6-A3BD-4E9D-A6A8-0F2596FD177F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4410" xr2:uid="{9890E2C9-68FC-4E17-9560-E34A85D78A5C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4410"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Schematic Reference Number</t>
   </si>
@@ -51,9 +50,6 @@
   </si>
   <si>
     <t>Total</t>
-  </si>
-  <si>
-    <t>Leak Sensor Bill of Materials</t>
   </si>
   <si>
     <t>CONN HEADER GH SIDE 2POS 1.25MM</t>
@@ -89,7 +85,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
@@ -118,7 +114,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -141,12 +137,108 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -156,15 +248,300 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="18">
+    <dxf>
+      <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="12" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -175,6 +552,24 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G5" totalsRowCount="1" headerRowDxfId="7" headerRowBorderDxfId="16" tableBorderDxfId="17" totalsRowBorderDxfId="15">
+  <autoFilter ref="A1:G5"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Schematic Reference Number" totalsRowLabel="Total" dataDxfId="14" totalsRowDxfId="6"/>
+    <tableColumn id="2" name="Part Description" dataDxfId="13" totalsRowDxfId="5"/>
+    <tableColumn id="3" name="Manufacturer Part Number" dataDxfId="12" totalsRowDxfId="4"/>
+    <tableColumn id="4" name="Datasheet" dataDxfId="11" totalsRowDxfId="3" dataCellStyle="Hyperlink"/>
+    <tableColumn id="5" name="Price" dataDxfId="10" totalsRowDxfId="2"/>
+    <tableColumn id="6" name="Quantity" dataDxfId="9" totalsRowDxfId="1"/>
+    <tableColumn id="7" name="Total" totalsRowFunction="custom" dataDxfId="8" totalsRowDxfId="0">
+      <totalsRowFormula>SUM(G2:G4)</totalsRowFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -473,136 +868,139 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA0C4221-2D67-4084-B811-A6255CF368A2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" customWidth="1"/>
     <col min="2" max="2" width="36.28515625" customWidth="1"/>
-    <col min="3" max="3" width="26.5703125" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="11.85546875" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
+      <c r="A2" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="F2" s="4">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>6</v>
+      <c r="G2" s="6">
+        <v>0.65</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>10</v>
-      </c>
       <c r="E3" s="3">
-        <v>0.65</v>
+        <v>0.52</v>
       </c>
       <c r="F3" s="4">
         <v>1</v>
       </c>
-      <c r="G3" s="3">
-        <v>0.65</v>
+      <c r="G3" s="6">
+        <v>0.52</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="A4" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0.52</v>
-      </c>
-      <c r="F4" s="4">
+      <c r="C4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="13">
+        <v>0.15</v>
+      </c>
+      <c r="F4" s="14">
         <v>1</v>
       </c>
-      <c r="G4" s="3">
-        <v>0.52</v>
+      <c r="G4" s="15">
+        <v>0.15</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="3">
-        <v>0.15</v>
-      </c>
-      <c r="F5" s="4">
-        <v>1</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0.15</v>
+      <c r="A5" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="15">
+        <f>SUM(G2:G4)</f>
+        <v>1.3199999999999998</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
-  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1" xr:uid="{174CED47-BA0F-4335-B9B7-2EDBD9AEB793}"/>
-    <hyperlink ref="D4" r:id="rId2" xr:uid="{42EFB3E7-30D5-4203-B5E1-602C9B09E756}"/>
-    <hyperlink ref="D5" r:id="rId3" xr:uid="{D5F8B79E-9AB2-497B-9457-F48D503CC468}"/>
+    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId2"/>
+    <hyperlink ref="D4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
+  <tableParts count="1">
+    <tablePart r:id="rId5"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>